<commit_message>
Add direct cpi and calculated cpi to data.xlsx
</commit_message>
<xml_diff>
--- a/Caches/output/data.xlsx
+++ b/Caches/output/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,16 @@
           <t>L2 Miss Rate</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Direct CPI</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated CPI</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -483,6 +493,12 @@
       <c r="F2" t="n">
         <v>0.001992</v>
       </c>
+      <c r="G2" t="n">
+        <v>5.036522</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.042728</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -507,6 +523,12 @@
       <c r="F3" t="n">
         <v>0.007042</v>
       </c>
+      <c r="G3" t="n">
+        <v>4.160849</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.021555</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -531,6 +553,12 @@
       <c r="F4" t="n">
         <v>0.026972</v>
       </c>
+      <c r="G4" t="n">
+        <v>3.905553</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.033842</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -555,6 +583,12 @@
       <c r="F5" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G5" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -579,6 +613,12 @@
       <c r="F6" t="n">
         <v>0.02954</v>
       </c>
+      <c r="G6" t="n">
+        <v>3.897679</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.036175</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -603,6 +643,12 @@
       <c r="F7" t="n">
         <v>0.029869</v>
       </c>
+      <c r="G7" t="n">
+        <v>3.896822</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.036477</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -627,6 +673,12 @@
       <c r="F8" t="n">
         <v>0.029885</v>
       </c>
+      <c r="G8" t="n">
+        <v>3.896752</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.036492</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -651,6 +703,12 @@
       <c r="F9" t="n">
         <v>0.029954</v>
       </c>
+      <c r="G9" t="n">
+        <v>3.896616</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.036555</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -675,6 +733,12 @@
       <c r="F10" t="n">
         <v>0.002747</v>
       </c>
+      <c r="G10" t="n">
+        <v>4.753193</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.074854</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -699,6 +763,12 @@
       <c r="F11" t="n">
         <v>0.006878</v>
       </c>
+      <c r="G11" t="n">
+        <v>4.178524</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.03553</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -723,6 +793,12 @@
       <c r="F12" t="n">
         <v>0.014669</v>
       </c>
+      <c r="G12" t="n">
+        <v>3.98374</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.027977</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -747,6 +823,12 @@
       <c r="F13" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G13" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -771,6 +853,12 @@
       <c r="F14" t="n">
         <v>0.039228</v>
       </c>
+      <c r="G14" t="n">
+        <v>3.876813</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.044055</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -795,6 +883,12 @@
       <c r="F15" t="n">
         <v>0.070948</v>
       </c>
+      <c r="G15" t="n">
+        <v>3.849235</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.07351</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -819,6 +913,12 @@
       <c r="F16" t="n">
         <v>0.088708</v>
       </c>
+      <c r="G16" t="n">
+        <v>3.842645</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.090709</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -843,6 +943,12 @@
       <c r="F17" t="n">
         <v>0.154588</v>
       </c>
+      <c r="G17" t="n">
+        <v>3.831575</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.155634</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -867,6 +973,12 @@
       <c r="F18" t="n">
         <v>0.029158</v>
       </c>
+      <c r="G18" t="n">
+        <v>3.900918</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.035878</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -891,6 +1003,12 @@
       <c r="F19" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G19" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -915,6 +1033,12 @@
       <c r="F20" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G20" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -939,6 +1063,12 @@
       <c r="F21" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G21" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -963,6 +1093,12 @@
       <c r="F22" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G22" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -987,6 +1123,12 @@
       <c r="F23" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G23" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1011,6 +1153,12 @@
       <c r="F24" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G24" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1035,6 +1183,12 @@
       <c r="F25" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G25" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1059,6 +1213,12 @@
       <c r="F26" t="n">
         <v>0.042334</v>
       </c>
+      <c r="G26" t="n">
+        <v>4.168985</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.065469</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1083,6 +1243,12 @@
       <c r="F27" t="n">
         <v>0.04938</v>
       </c>
+      <c r="G27" t="n">
+        <v>4.026669</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1.063076</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1107,6 +1273,12 @@
       <c r="F28" t="n">
         <v>0.042902</v>
       </c>
+      <c r="G28" t="n">
+        <v>3.932666</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.051251</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1131,6 +1303,12 @@
       <c r="F29" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G29" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1155,6 +1333,12 @@
       <c r="F30" t="n">
         <v>0.013859</v>
       </c>
+      <c r="G30" t="n">
+        <v>3.905948</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.021406</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1179,6 +1363,12 @@
       <c r="F31" t="n">
         <v>0.00533</v>
       </c>
+      <c r="G31" t="n">
+        <v>3.947798</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1.016099</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1203,6 +1393,12 @@
       <c r="F32" t="n">
         <v>0.001492</v>
       </c>
+      <c r="G32" t="n">
+        <v>4.105177</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1.023663</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1227,6 +1423,12 @@
       <c r="F33" t="n">
         <v>0.02706</v>
       </c>
+      <c r="G33" t="n">
+        <v>3.905159</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1.033921</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1251,6 +1453,12 @@
       <c r="F34" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G34" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1275,6 +1483,12 @@
       <c r="F35" t="n">
         <v>0.028724</v>
       </c>
+      <c r="G35" t="n">
+        <v>3.900079</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1.035429</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1299,6 +1513,12 @@
       <c r="F36" t="n">
         <v>0.028773</v>
       </c>
+      <c r="G36" t="n">
+        <v>3.899845</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1.035474</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1323,6 +1543,12 @@
       <c r="F37" t="n">
         <v>0.004803</v>
       </c>
+      <c r="G37" t="n">
+        <v>4.370536</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1.04594</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1347,6 +1573,12 @@
       <c r="F38" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G38" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1371,6 +1603,12 @@
       <c r="F39" t="n">
         <v>0.059732</v>
       </c>
+      <c r="G39" t="n">
+        <v>3.855532</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1.06282</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1395,6 +1633,12 @@
       <c r="F40" t="n">
         <v>0.06245</v>
       </c>
+      <c r="G40" t="n">
+        <v>3.853747</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1.065393</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1419,6 +1663,12 @@
       <c r="F41" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G41" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1443,6 +1693,12 @@
       <c r="F42" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G42" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1467,6 +1723,12 @@
       <c r="F43" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G43" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1491,6 +1753,12 @@
       <c r="F44" t="n">
         <v>0.028555</v>
       </c>
+      <c r="G44" t="n">
+        <v>3.900594</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1.035275</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1515,6 +1783,12 @@
       <c r="F45" t="n">
         <v>0.998317</v>
       </c>
+      <c r="G45" t="n">
+        <v>26.024219</v>
+      </c>
+      <c r="H45" t="n">
+        <v>2.119923</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1539,6 +1813,12 @@
       <c r="F46" t="n">
         <v>0.998686</v>
       </c>
+      <c r="G46" t="n">
+        <v>26.037528</v>
+      </c>
+      <c r="H46" t="n">
+        <v>2.120258</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1563,6 +1843,12 @@
       <c r="F47" t="n">
         <v>0.999136</v>
       </c>
+      <c r="G47" t="n">
+        <v>26.030926</v>
+      </c>
+      <c r="H47" t="n">
+        <v>2.120666</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1587,6 +1873,12 @@
       <c r="F48" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G48" t="n">
+        <v>26.019584</v>
+      </c>
+      <c r="H48" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1611,6 +1903,12 @@
       <c r="F49" t="n">
         <v>0.999723</v>
       </c>
+      <c r="G49" t="n">
+        <v>26.014169</v>
+      </c>
+      <c r="H49" t="n">
+        <v>2.121198</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1635,6 +1933,12 @@
       <c r="F50" t="n">
         <v>0.9998</v>
       </c>
+      <c r="G50" t="n">
+        <v>26.006216</v>
+      </c>
+      <c r="H50" t="n">
+        <v>2.121268</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1659,6 +1963,12 @@
       <c r="F51" t="n">
         <v>0.999814</v>
       </c>
+      <c r="G51" t="n">
+        <v>26.033599</v>
+      </c>
+      <c r="H51" t="n">
+        <v>2.12128</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1683,6 +1993,12 @@
       <c r="F52" t="n">
         <v>0.999816</v>
       </c>
+      <c r="G52" t="n">
+        <v>26.0345</v>
+      </c>
+      <c r="H52" t="n">
+        <v>2.121282</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1707,6 +2023,12 @@
       <c r="F53" t="n">
         <v>0.976305</v>
       </c>
+      <c r="G53" t="n">
+        <v>26.10692</v>
+      </c>
+      <c r="H53" t="n">
+        <v>2.100689</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1731,6 +2053,12 @@
       <c r="F54" t="n">
         <v>0.993957</v>
       </c>
+      <c r="G54" t="n">
+        <v>26.034201</v>
+      </c>
+      <c r="H54" t="n">
+        <v>2.116132</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1755,6 +2083,12 @@
       <c r="F55" t="n">
         <v>0.998058</v>
       </c>
+      <c r="G55" t="n">
+        <v>26.042438</v>
+      </c>
+      <c r="H55" t="n">
+        <v>2.119731</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1779,6 +2113,12 @@
       <c r="F56" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G56" t="n">
+        <v>26.019584</v>
+      </c>
+      <c r="H56" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1803,6 +2143,12 @@
       <c r="F57" t="n">
         <v>0.999687</v>
       </c>
+      <c r="G57" t="n">
+        <v>26.013784</v>
+      </c>
+      <c r="H57" t="n">
+        <v>2.121162</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1827,6 +2173,12 @@
       <c r="F58" t="n">
         <v>0.999691</v>
       </c>
+      <c r="G58" t="n">
+        <v>26.057559</v>
+      </c>
+      <c r="H58" t="n">
+        <v>2.121165</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1851,6 +2203,12 @@
       <c r="F59" t="n">
         <v>0.999692</v>
       </c>
+      <c r="G59" t="n">
+        <v>26.057559</v>
+      </c>
+      <c r="H59" t="n">
+        <v>2.121166</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1875,6 +2233,12 @@
       <c r="F60" t="n">
         <v>0.999694</v>
       </c>
+      <c r="G60" t="n">
+        <v>26.057559</v>
+      </c>
+      <c r="H60" t="n">
+        <v>2.121168</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1899,6 +2263,12 @@
       <c r="F61" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G61" t="n">
+        <v>26.060408</v>
+      </c>
+      <c r="H61" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1923,6 +2293,12 @@
       <c r="F62" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G62" t="n">
+        <v>26.010508</v>
+      </c>
+      <c r="H62" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1947,6 +2323,12 @@
       <c r="F63" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G63" t="n">
+        <v>26.0671</v>
+      </c>
+      <c r="H63" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1971,6 +2353,12 @@
       <c r="F64" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G64" t="n">
+        <v>26.019584</v>
+      </c>
+      <c r="H64" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1995,6 +2383,12 @@
       <c r="F65" t="n">
         <v>0.999517</v>
       </c>
+      <c r="G65" t="n">
+        <v>25.987687</v>
+      </c>
+      <c r="H65" t="n">
+        <v>2.121012</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2019,6 +2413,12 @@
       <c r="F66" t="n">
         <v>0.999517</v>
       </c>
+      <c r="G66" t="n">
+        <v>25.92413</v>
+      </c>
+      <c r="H66" t="n">
+        <v>2.121012</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2043,6 +2443,12 @@
       <c r="F67" t="n">
         <v>0.999514</v>
       </c>
+      <c r="G67" t="n">
+        <v>25.807272</v>
+      </c>
+      <c r="H67" t="n">
+        <v>2.121009</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2067,6 +2473,12 @@
       <c r="F68" t="n">
         <v>0.818064</v>
       </c>
+      <c r="G68" t="n">
+        <v>22.24489</v>
+      </c>
+      <c r="H68" t="n">
+        <v>1.939559</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2091,6 +2503,12 @@
       <c r="F69" t="n">
         <v>0.812459</v>
       </c>
+      <c r="G69" t="n">
+        <v>67.242693</v>
+      </c>
+      <c r="H69" t="n">
+        <v>2.78396</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2115,6 +2533,12 @@
       <c r="F70" t="n">
         <v>0.999853</v>
       </c>
+      <c r="G70" t="n">
+        <v>84.26831300000001</v>
+      </c>
+      <c r="H70" t="n">
+        <v>2.485646</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2139,6 +2563,12 @@
       <c r="F71" t="n">
         <v>0.999797</v>
       </c>
+      <c r="G71" t="n">
+        <v>45.530116</v>
+      </c>
+      <c r="H71" t="n">
+        <v>2.242712</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2163,6 +2593,12 @@
       <c r="F72" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G72" t="n">
+        <v>26.019584</v>
+      </c>
+      <c r="H72" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2187,6 +2623,12 @@
       <c r="F73" t="n">
         <v>0.998335</v>
       </c>
+      <c r="G73" t="n">
+        <v>16.903227</v>
+      </c>
+      <c r="H73" t="n">
+        <v>2.059153</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2211,6 +2653,12 @@
       <c r="F74" t="n">
         <v>0.992438</v>
       </c>
+      <c r="G74" t="n">
+        <v>12.882278</v>
+      </c>
+      <c r="H74" t="n">
+        <v>2.023028</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2235,6 +2683,12 @@
       <c r="F75" t="n">
         <v>0.917967</v>
       </c>
+      <c r="G75" t="n">
+        <v>9.523178</v>
+      </c>
+      <c r="H75" t="n">
+        <v>1.934502</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2259,6 +2713,12 @@
       <c r="F76" t="n">
         <v>0.999377</v>
       </c>
+      <c r="G76" t="n">
+        <v>26.010164</v>
+      </c>
+      <c r="H76" t="n">
+        <v>2.120884</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2283,6 +2743,12 @@
       <c r="F77" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G77" t="n">
+        <v>26.019584</v>
+      </c>
+      <c r="H77" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2307,6 +2773,12 @@
       <c r="F78" t="n">
         <v>0.9996390000000001</v>
       </c>
+      <c r="G78" t="n">
+        <v>26.029681</v>
+      </c>
+      <c r="H78" t="n">
+        <v>2.121122</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2331,6 +2803,12 @@
       <c r="F79" t="n">
         <v>0.99977</v>
       </c>
+      <c r="G79" t="n">
+        <v>26.030053</v>
+      </c>
+      <c r="H79" t="n">
+        <v>2.121241</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2355,6 +2833,12 @@
       <c r="F80" t="n">
         <v>0.996798</v>
       </c>
+      <c r="G80" t="n">
+        <v>26.040118</v>
+      </c>
+      <c r="H80" t="n">
+        <v>2.118625</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2379,6 +2863,12 @@
       <c r="F81" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G81" t="n">
+        <v>26.019584</v>
+      </c>
+      <c r="H81" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2403,6 +2893,12 @@
       <c r="F82" t="n">
         <v>0.99968</v>
       </c>
+      <c r="G82" t="n">
+        <v>26.016276</v>
+      </c>
+      <c r="H82" t="n">
+        <v>2.121156</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2427,6 +2923,12 @@
       <c r="F83" t="n">
         <v>0.999681</v>
       </c>
+      <c r="G83" t="n">
+        <v>26.016276</v>
+      </c>
+      <c r="H83" t="n">
+        <v>2.121157</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2451,6 +2953,12 @@
       <c r="F84" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G84" t="n">
+        <v>25.994884</v>
+      </c>
+      <c r="H84" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2475,6 +2983,12 @@
       <c r="F85" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G85" t="n">
+        <v>26.019584</v>
+      </c>
+      <c r="H85" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2499,6 +3013,12 @@
       <c r="F86" t="n">
         <v>0.999518</v>
       </c>
+      <c r="G86" t="n">
+        <v>26.058949</v>
+      </c>
+      <c r="H86" t="n">
+        <v>2.121013</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2522,6 +3042,12 @@
       </c>
       <c r="F87" t="n">
         <v>0.999518</v>
+      </c>
+      <c r="G87" t="n">
+        <v>26.027728</v>
+      </c>
+      <c r="H87" t="n">
+        <v>2.121013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add miss latency CPI to data.xlsx
</commit_message>
<xml_diff>
--- a/Caches/output/data.xlsx
+++ b/Caches/output/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Calculated CPI</t>
+          <t>CPI using Miss Rate</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>CPI using Miss Ticks</t>
         </is>
       </c>
     </row>
@@ -499,6 +504,9 @@
       <c r="H2" t="n">
         <v>1.042728</v>
       </c>
+      <c r="I2" t="n">
+        <v>1.019088819932465</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -529,6 +537,9 @@
       <c r="H3" t="n">
         <v>1.021555</v>
       </c>
+      <c r="I3" t="n">
+        <v>1.023137235539063</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -559,6 +570,9 @@
       <c r="H4" t="n">
         <v>1.033842</v>
       </c>
+      <c r="I4" t="n">
+        <v>1.024614725353648</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -589,6 +603,9 @@
       <c r="H5" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I5" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -619,6 +636,9 @@
       <c r="H6" t="n">
         <v>1.036175</v>
       </c>
+      <c r="I6" t="n">
+        <v>1.024672631043375</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -649,6 +669,9 @@
       <c r="H7" t="n">
         <v>1.036477</v>
       </c>
+      <c r="I7" t="n">
+        <v>1.024682641962886</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -679,6 +702,9 @@
       <c r="H8" t="n">
         <v>1.036492</v>
       </c>
+      <c r="I8" t="n">
+        <v>1.024676198087543</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -709,6 +735,9 @@
       <c r="H9" t="n">
         <v>1.036555</v>
       </c>
+      <c r="I9" t="n">
+        <v>1.024689347653919</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -739,6 +768,9 @@
       <c r="H10" t="n">
         <v>1.074854</v>
       </c>
+      <c r="I10" t="n">
+        <v>1.213642583497051</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -769,6 +801,9 @@
       <c r="H11" t="n">
         <v>1.03553</v>
       </c>
+      <c r="I11" t="n">
+        <v>1.094881339048007</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -799,6 +834,9 @@
       <c r="H12" t="n">
         <v>1.027977</v>
       </c>
+      <c r="I12" t="n">
+        <v>1.046702497419491</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -829,6 +867,9 @@
       <c r="H13" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I13" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -859,6 +900,9 @@
       <c r="H14" t="n">
         <v>1.044055</v>
       </c>
+      <c r="I14" t="n">
+        <v>1.01817412638853</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -889,6 +933,9 @@
       <c r="H15" t="n">
         <v>1.07351</v>
       </c>
+      <c r="I15" t="n">
+        <v>1.010547152178551</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -919,6 +966,9 @@
       <c r="H16" t="n">
         <v>1.090709</v>
       </c>
+      <c r="I16" t="n">
+        <v>1.008704953243769</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -949,6 +999,9 @@
       <c r="H17" t="n">
         <v>1.155634</v>
       </c>
+      <c r="I17" t="n">
+        <v>1.005610650822219</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -979,6 +1032,9 @@
       <c r="H18" t="n">
         <v>1.035878</v>
       </c>
+      <c r="I18" t="n">
+        <v>1.024710545718464</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1009,6 +1065,9 @@
       <c r="H19" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I19" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1039,6 +1098,9 @@
       <c r="H20" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I20" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1069,6 +1131,9 @@
       <c r="H21" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I21" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1099,6 +1164,9 @@
       <c r="H22" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I22" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1129,6 +1197,9 @@
       <c r="H23" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I23" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1159,6 +1230,9 @@
       <c r="H24" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I24" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1189,6 +1263,9 @@
       <c r="H25" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I25" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1219,6 +1296,9 @@
       <c r="H26" t="n">
         <v>1.065469</v>
       </c>
+      <c r="I26" t="n">
+        <v>1.083759814204811</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1249,6 +1329,9 @@
       <c r="H27" t="n">
         <v>1.063076</v>
       </c>
+      <c r="I27" t="n">
+        <v>1.052942910123217</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1279,6 +1362,9 @@
       <c r="H28" t="n">
         <v>1.051251</v>
       </c>
+      <c r="I28" t="n">
+        <v>1.031939664294966</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1309,6 +1395,9 @@
       <c r="H29" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I29" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1339,6 +1428,9 @@
       <c r="H30" t="n">
         <v>1.021406</v>
       </c>
+      <c r="I30" t="n">
+        <v>1.026492576786782</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1369,6 +1461,9 @@
       <c r="H31" t="n">
         <v>1.016099</v>
       </c>
+      <c r="I31" t="n">
+        <v>1.037541853663117</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1399,6 +1494,9 @@
       <c r="H32" t="n">
         <v>1.023663</v>
       </c>
+      <c r="I32" t="n">
+        <v>1.07572697587002</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1429,6 +1527,9 @@
       <c r="H33" t="n">
         <v>1.033921</v>
       </c>
+      <c r="I33" t="n">
+        <v>1.024610014196572</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1459,6 +1560,9 @@
       <c r="H34" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I34" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1489,6 +1593,9 @@
       <c r="H35" t="n">
         <v>1.035429</v>
       </c>
+      <c r="I35" t="n">
+        <v>1.024662076996317</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1519,6 +1626,9 @@
       <c r="H36" t="n">
         <v>1.035474</v>
       </c>
+      <c r="I36" t="n">
+        <v>1.024636785081533</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1549,6 +1659,9 @@
       <c r="H37" t="n">
         <v>1.04594</v>
       </c>
+      <c r="I37" t="n">
+        <v>1.137561197819615</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1579,6 +1692,9 @@
       <c r="H38" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I38" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1609,6 +1725,9 @@
       <c r="H39" t="n">
         <v>1.06282</v>
       </c>
+      <c r="I39" t="n">
+        <v>1.012298486563128</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1639,6 +1758,9 @@
       <c r="H40" t="n">
         <v>1.065393</v>
       </c>
+      <c r="I40" t="n">
+        <v>1.011800945835822</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1669,6 +1791,9 @@
       <c r="H41" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I41" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1699,6 +1824,9 @@
       <c r="H42" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I42" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1729,6 +1857,9 @@
       <c r="H43" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I43" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1759,6 +1890,9 @@
       <c r="H44" t="n">
         <v>1.035275</v>
       </c>
+      <c r="I44" t="n">
+        <v>1.024654752962982</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1789,6 +1923,9 @@
       <c r="H45" t="n">
         <v>2.119923</v>
       </c>
+      <c r="I45" t="n">
+        <v>1.818778183546783</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1819,6 +1956,9 @@
       <c r="H46" t="n">
         <v>2.120258</v>
       </c>
+      <c r="I46" t="n">
+        <v>1.818914285413227</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1849,6 +1989,9 @@
       <c r="H47" t="n">
         <v>2.120666</v>
       </c>
+      <c r="I47" t="n">
+        <v>1.818924458847237</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1879,6 +2022,9 @@
       <c r="H48" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I48" t="n">
+        <v>1.818893596775429</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1909,6 +2055,9 @@
       <c r="H49" t="n">
         <v>2.121198</v>
       </c>
+      <c r="I49" t="n">
+        <v>1.818884338046038</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1939,6 +2088,9 @@
       <c r="H50" t="n">
         <v>2.121268</v>
       </c>
+      <c r="I50" t="n">
+        <v>1.818846553453971</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1969,6 +2121,9 @@
       <c r="H51" t="n">
         <v>2.12128</v>
       </c>
+      <c r="I51" t="n">
+        <v>1.819041641142949</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1999,6 +2154,9 @@
       <c r="H52" t="n">
         <v>2.121282</v>
       </c>
+      <c r="I52" t="n">
+        <v>1.819049030194306</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2029,6 +2187,9 @@
       <c r="H53" t="n">
         <v>2.100689</v>
       </c>
+      <c r="I53" t="n">
+        <v>1.819736066944585</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2059,6 +2220,9 @@
       <c r="H54" t="n">
         <v>2.116132</v>
       </c>
+      <c r="I54" t="n">
+        <v>1.819053449046702</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2089,6 +2253,9 @@
       <c r="H55" t="n">
         <v>2.119731</v>
       </c>
+      <c r="I55" t="n">
+        <v>1.819066683280637</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2119,6 +2286,9 @@
       <c r="H56" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I56" t="n">
+        <v>1.818893596775429</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2149,6 +2319,9 @@
       <c r="H57" t="n">
         <v>2.121162</v>
       </c>
+      <c r="I57" t="n">
+        <v>1.818851959404859</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2179,6 +2352,9 @@
       <c r="H58" t="n">
         <v>2.121165</v>
       </c>
+      <c r="I58" t="n">
+        <v>1.819156605316266</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2209,6 +2385,9 @@
       <c r="H59" t="n">
         <v>2.121166</v>
       </c>
+      <c r="I59" t="n">
+        <v>1.819156556194362</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2239,6 +2418,9 @@
       <c r="H60" t="n">
         <v>2.121168</v>
       </c>
+      <c r="I60" t="n">
+        <v>1.819156538541178</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2269,6 +2451,9 @@
       <c r="H61" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I61" t="n">
+        <v>1.819178433184797</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2299,6 +2484,9 @@
       <c r="H62" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I62" t="n">
+        <v>1.818831369699976</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2329,6 +2517,9 @@
       <c r="H63" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I63" t="n">
+        <v>1.819225379348832</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2359,6 +2550,9 @@
       <c r="H64" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I64" t="n">
+        <v>1.818893596775429</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2389,6 +2583,9 @@
       <c r="H65" t="n">
         <v>2.121012</v>
       </c>
+      <c r="I65" t="n">
+        <v>1.818672046427031</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2419,6 +2616,9 @@
       <c r="H66" t="n">
         <v>2.121012</v>
       </c>
+      <c r="I66" t="n">
+        <v>1.818226414992708</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2449,6 +2649,9 @@
       <c r="H67" t="n">
         <v>2.121009</v>
       </c>
+      <c r="I67" t="n">
+        <v>1.817404032428819</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2479,6 +2682,9 @@
       <c r="H68" t="n">
         <v>1.939559</v>
       </c>
+      <c r="I68" t="n">
+        <v>1.788163666731069</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2509,6 +2715,9 @@
       <c r="H69" t="n">
         <v>2.78396</v>
       </c>
+      <c r="I69" t="n">
+        <v>1.956703954345838</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2539,6 +2748,9 @@
       <c r="H70" t="n">
         <v>2.485646</v>
       </c>
+      <c r="I70" t="n">
+        <v>1.953237169491113</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2569,6 +2781,9 @@
       <c r="H71" t="n">
         <v>2.242712</v>
       </c>
+      <c r="I71" t="n">
+        <v>1.902151521661942</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2599,6 +2814,9 @@
       <c r="H72" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I72" t="n">
+        <v>1.818893596775429</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2629,6 +2847,9 @@
       <c r="H73" t="n">
         <v>2.059153</v>
       </c>
+      <c r="I73" t="n">
+        <v>1.713588805558187</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2659,6 +2880,9 @@
       <c r="H74" t="n">
         <v>2.023028</v>
       </c>
+      <c r="I74" t="n">
+        <v>1.619220111036396</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2689,6 +2913,9 @@
       <c r="H75" t="n">
         <v>1.934502</v>
       </c>
+      <c r="I75" t="n">
+        <v>1.48165700843835</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2719,6 +2946,9 @@
       <c r="H76" t="n">
         <v>2.120884</v>
       </c>
+      <c r="I76" t="n">
+        <v>1.818813880125368</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2749,6 +2979,9 @@
       <c r="H77" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I77" t="n">
+        <v>1.818893596775429</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2779,6 +3012,9 @@
       <c r="H78" t="n">
         <v>2.121122</v>
       </c>
+      <c r="I78" t="n">
+        <v>1.818978096568205</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2809,6 +3045,9 @@
       <c r="H79" t="n">
         <v>2.121241</v>
       </c>
+      <c r="I79" t="n">
+        <v>1.818998541685307</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2839,6 +3078,9 @@
       <c r="H80" t="n">
         <v>2.118625</v>
       </c>
+      <c r="I80" t="n">
+        <v>1.819064990520892</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2869,6 +3111,9 @@
       <c r="H81" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I81" t="n">
+        <v>1.818893596775429</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2899,6 +3144,9 @@
       <c r="H82" t="n">
         <v>2.121156</v>
       </c>
+      <c r="I82" t="n">
+        <v>1.818869442566909</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2929,6 +3177,9 @@
       <c r="H83" t="n">
         <v>2.121157</v>
       </c>
+      <c r="I83" t="n">
+        <v>1.818869755447212</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2959,6 +3210,9 @@
       <c r="H84" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I84" t="n">
+        <v>1.818722761707717</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2989,6 +3243,9 @@
       <c r="H85" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I85" t="n">
+        <v>1.818893596775429</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -3019,6 +3276,9 @@
       <c r="H86" t="n">
         <v>2.121013</v>
       </c>
+      <c r="I86" t="n">
+        <v>1.819168757390788</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -3048,6 +3308,9 @@
       </c>
       <c r="H87" t="n">
         <v>2.121013</v>
+      </c>
+      <c r="I87" t="n">
+        <v>1.818951804196615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix miss latency calculation
</commit_message>
<xml_diff>
--- a/Caches/output/data.xlsx
+++ b/Caches/output/data.xlsx
@@ -505,7 +505,7 @@
         <v>1.042728</v>
       </c>
       <c r="I2" t="n">
-        <v>1.019088819932465</v>
+        <v>1.04807073996</v>
       </c>
     </row>
     <row r="3">
@@ -538,7 +538,7 @@
         <v>1.021555</v>
       </c>
       <c r="I3" t="n">
-        <v>1.023137235539063</v>
+        <v>1.04813537996</v>
       </c>
     </row>
     <row r="4">
@@ -571,7 +571,7 @@
         <v>1.033842</v>
       </c>
       <c r="I4" t="n">
-        <v>1.024614725353648</v>
+        <v>1.04806716996</v>
       </c>
     </row>
     <row r="5">
@@ -604,7 +604,7 @@
         <v>1.035275</v>
       </c>
       <c r="I5" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="6">
@@ -637,7 +637,7 @@
         <v>1.036175</v>
       </c>
       <c r="I6" t="n">
-        <v>1.024672631043375</v>
+        <v>1.04808310996</v>
       </c>
     </row>
     <row r="7">
@@ -670,7 +670,7 @@
         <v>1.036477</v>
       </c>
       <c r="I7" t="n">
-        <v>1.024682641962886</v>
+        <v>1.04809203996</v>
       </c>
     </row>
     <row r="8">
@@ -703,7 +703,7 @@
         <v>1.036492</v>
       </c>
       <c r="I8" t="n">
-        <v>1.024676198087543</v>
+        <v>1.04807861996</v>
       </c>
     </row>
     <row r="9">
@@ -736,7 +736,7 @@
         <v>1.036555</v>
       </c>
       <c r="I9" t="n">
-        <v>1.024689347653919</v>
+        <v>1.04810255996</v>
       </c>
     </row>
     <row r="10">
@@ -769,7 +769,7 @@
         <v>1.074854</v>
       </c>
       <c r="I10" t="n">
-        <v>1.213642583497051</v>
+        <v>1.50774336986</v>
       </c>
     </row>
     <row r="11">
@@ -802,7 +802,7 @@
         <v>1.03553</v>
       </c>
       <c r="I11" t="n">
-        <v>1.094881339048007</v>
+        <v>1.19823244964</v>
       </c>
     </row>
     <row r="12">
@@ -835,7 +835,7 @@
         <v>1.027977</v>
       </c>
       <c r="I12" t="n">
-        <v>1.046702497419491</v>
+        <v>1.09302550996</v>
       </c>
     </row>
     <row r="13">
@@ -868,7 +868,7 @@
         <v>1.035275</v>
       </c>
       <c r="I13" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="14">
@@ -901,7 +901,7 @@
         <v>1.044055</v>
       </c>
       <c r="I14" t="n">
-        <v>1.01817412638853</v>
+        <v>1.03522892996</v>
       </c>
     </row>
     <row r="15">
@@ -934,7 +934,7 @@
         <v>1.07351</v>
       </c>
       <c r="I15" t="n">
-        <v>1.010547152178551</v>
+        <v>1.02029927996</v>
       </c>
     </row>
     <row r="16">
@@ -967,7 +967,7 @@
         <v>1.090709</v>
       </c>
       <c r="I16" t="n">
-        <v>1.008704953243769</v>
+        <v>1.01672505996</v>
       </c>
     </row>
     <row r="17">
@@ -1000,7 +1000,7 @@
         <v>1.155634</v>
       </c>
       <c r="I17" t="n">
-        <v>1.005610650822219</v>
+        <v>1.01074883996</v>
       </c>
     </row>
     <row r="18">
@@ -1033,7 +1033,7 @@
         <v>1.035878</v>
       </c>
       <c r="I18" t="n">
-        <v>1.024710545718464</v>
+        <v>1.04819701996</v>
       </c>
     </row>
     <row r="19">
@@ -1066,7 +1066,7 @@
         <v>1.035275</v>
       </c>
       <c r="I19" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="20">
@@ -1099,7 +1099,7 @@
         <v>1.035275</v>
       </c>
       <c r="I20" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="21">
@@ -1132,7 +1132,7 @@
         <v>1.035275</v>
       </c>
       <c r="I21" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="22">
@@ -1165,7 +1165,7 @@
         <v>1.035275</v>
       </c>
       <c r="I22" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="23">
@@ -1198,7 +1198,7 @@
         <v>1.035275</v>
       </c>
       <c r="I23" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="24">
@@ -1231,7 +1231,7 @@
         <v>1.035275</v>
       </c>
       <c r="I24" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="25">
@@ -1264,7 +1264,7 @@
         <v>1.035275</v>
       </c>
       <c r="I25" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="26">
@@ -1297,7 +1297,7 @@
         <v>1.065469</v>
       </c>
       <c r="I26" t="n">
-        <v>1.083759814204811</v>
+        <v>1.17459711996</v>
       </c>
     </row>
     <row r="27">
@@ -1330,7 +1330,7 @@
         <v>1.063076</v>
       </c>
       <c r="I27" t="n">
-        <v>1.052942910123217</v>
+        <v>1.10659202996</v>
       </c>
     </row>
     <row r="28">
@@ -1363,7 +1363,7 @@
         <v>1.051251</v>
       </c>
       <c r="I28" t="n">
-        <v>1.031939664294966</v>
+        <v>1.06280415996</v>
       </c>
     </row>
     <row r="29">
@@ -1396,7 +1396,7 @@
         <v>1.035275</v>
       </c>
       <c r="I29" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="30">
@@ -1429,7 +1429,7 @@
         <v>1.021406</v>
       </c>
       <c r="I30" t="n">
-        <v>1.026492576786782</v>
+        <v>1.05173942996</v>
       </c>
     </row>
     <row r="31">
@@ -1462,7 +1462,7 @@
         <v>1.016099</v>
       </c>
       <c r="I31" t="n">
-        <v>1.037541853663117</v>
+        <v>1.07410398996</v>
       </c>
     </row>
     <row r="32">
@@ -1495,7 +1495,7 @@
         <v>1.023663</v>
       </c>
       <c r="I32" t="n">
-        <v>1.07572697587002</v>
+        <v>1.15543669996</v>
       </c>
     </row>
     <row r="33">
@@ -1528,7 +1528,7 @@
         <v>1.033921</v>
       </c>
       <c r="I33" t="n">
-        <v>1.024610014196572</v>
+        <v>1.04805311996</v>
       </c>
     </row>
     <row r="34">
@@ -1561,7 +1561,7 @@
         <v>1.035275</v>
       </c>
       <c r="I34" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="35">
@@ -1594,7 +1594,7 @@
         <v>1.035429</v>
       </c>
       <c r="I35" t="n">
-        <v>1.024662076996317</v>
+        <v>1.04809213996</v>
       </c>
     </row>
     <row r="36">
@@ -1627,7 +1627,7 @@
         <v>1.035474</v>
       </c>
       <c r="I36" t="n">
-        <v>1.024636785081533</v>
+        <v>1.04803992996</v>
       </c>
     </row>
     <row r="37">
@@ -1660,7 +1660,7 @@
         <v>1.04594</v>
       </c>
       <c r="I37" t="n">
-        <v>1.137561197819615</v>
+        <v>1.30060880996</v>
       </c>
     </row>
     <row r="38">
@@ -1693,7 +1693,7 @@
         <v>1.035275</v>
       </c>
       <c r="I38" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="39">
@@ -1726,7 +1726,7 @@
         <v>1.06282</v>
       </c>
       <c r="I39" t="n">
-        <v>1.012298486563128</v>
+        <v>1.02370865996</v>
       </c>
     </row>
     <row r="40">
@@ -1759,7 +1759,7 @@
         <v>1.065393</v>
       </c>
       <c r="I40" t="n">
-        <v>1.011800945835822</v>
+        <v>1.02273897996</v>
       </c>
     </row>
     <row r="41">
@@ -1792,7 +1792,7 @@
         <v>1.035275</v>
       </c>
       <c r="I41" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="42">
@@ -1825,7 +1825,7 @@
         <v>1.035275</v>
       </c>
       <c r="I42" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="43">
@@ -1858,7 +1858,7 @@
         <v>1.035275</v>
       </c>
       <c r="I43" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="44">
@@ -1891,7 +1891,7 @@
         <v>1.035275</v>
       </c>
       <c r="I44" t="n">
-        <v>1.024654752962982</v>
+        <v>1.04808419996</v>
       </c>
     </row>
     <row r="45">
@@ -1924,7 +1924,7 @@
         <v>2.119923</v>
       </c>
       <c r="I45" t="n">
-        <v>1.818778183546783</v>
+        <v>11.65405681996</v>
       </c>
     </row>
     <row r="46">
@@ -1957,7 +1957,7 @@
         <v>2.120258</v>
       </c>
       <c r="I46" t="n">
-        <v>1.818914285413227</v>
+        <v>11.66127735996</v>
       </c>
     </row>
     <row r="47">
@@ -1990,7 +1990,7 @@
         <v>2.120666</v>
       </c>
       <c r="I47" t="n">
-        <v>1.818924458847237</v>
+        <v>11.65870669996</v>
       </c>
     </row>
     <row r="48">
@@ -2023,7 +2023,7 @@
         <v>2.121013</v>
       </c>
       <c r="I48" t="n">
-        <v>1.818893596775429</v>
+        <v>11.65366083996</v>
       </c>
     </row>
     <row r="49">
@@ -2056,7 +2056,7 @@
         <v>2.121198</v>
       </c>
       <c r="I49" t="n">
-        <v>1.818884338046038</v>
+        <v>11.65132341996</v>
       </c>
     </row>
     <row r="50">
@@ -2089,7 +2089,7 @@
         <v>2.121268</v>
       </c>
       <c r="I50" t="n">
-        <v>1.818846553453971</v>
+        <v>11.64757588996</v>
       </c>
     </row>
     <row r="51">
@@ -2122,7 +2122,7 @@
         <v>2.12128</v>
       </c>
       <c r="I51" t="n">
-        <v>1.819041641142949</v>
+        <v>11.66132641996</v>
       </c>
     </row>
     <row r="52">
@@ -2155,7 +2155,7 @@
         <v>2.121282</v>
       </c>
       <c r="I52" t="n">
-        <v>1.819049030194306</v>
+        <v>11.66179159996</v>
       </c>
     </row>
     <row r="53">
@@ -2188,7 +2188,7 @@
         <v>2.100689</v>
       </c>
       <c r="I53" t="n">
-        <v>1.819736066944585</v>
+        <v>11.70041760996</v>
       </c>
     </row>
     <row r="54">
@@ -2221,7 +2221,7 @@
         <v>2.116132</v>
       </c>
       <c r="I54" t="n">
-        <v>1.819053449046702</v>
+        <v>11.66172645996</v>
       </c>
     </row>
     <row r="55">
@@ -2254,7 +2254,7 @@
         <v>2.119731</v>
       </c>
       <c r="I55" t="n">
-        <v>1.819066683280637</v>
+        <v>11.66527231996</v>
       </c>
     </row>
     <row r="56">
@@ -2287,7 +2287,7 @@
         <v>2.121013</v>
       </c>
       <c r="I56" t="n">
-        <v>1.818893596775429</v>
+        <v>11.65366083996</v>
       </c>
     </row>
     <row r="57">
@@ -2320,7 +2320,7 @@
         <v>2.121162</v>
       </c>
       <c r="I57" t="n">
-        <v>1.818851959404859</v>
+        <v>11.65074453996</v>
       </c>
     </row>
     <row r="58">
@@ -2353,7 +2353,7 @@
         <v>2.121165</v>
       </c>
       <c r="I58" t="n">
-        <v>1.819156605316266</v>
+        <v>11.67263649996</v>
       </c>
     </row>
     <row r="59">
@@ -2386,7 +2386,7 @@
         <v>2.121166</v>
       </c>
       <c r="I59" t="n">
-        <v>1.819156556194362</v>
+        <v>11.67263585996</v>
       </c>
     </row>
     <row r="60">
@@ -2419,7 +2419,7 @@
         <v>2.121168</v>
       </c>
       <c r="I60" t="n">
-        <v>1.819156538541178</v>
+        <v>11.67263562996</v>
       </c>
     </row>
     <row r="61">
@@ -2452,7 +2452,7 @@
         <v>2.121013</v>
       </c>
       <c r="I61" t="n">
-        <v>1.819178433184797</v>
+        <v>11.67408785996</v>
       </c>
     </row>
     <row r="62">
@@ -2485,7 +2485,7 @@
         <v>2.121013</v>
       </c>
       <c r="I62" t="n">
-        <v>1.818831369699976</v>
+        <v>11.64913541996</v>
       </c>
     </row>
     <row r="63">
@@ -2518,7 +2518,7 @@
         <v>2.121013</v>
       </c>
       <c r="I63" t="n">
-        <v>1.819225379348832</v>
+        <v>11.67744037996</v>
       </c>
     </row>
     <row r="64">
@@ -2551,7 +2551,7 @@
         <v>2.121013</v>
       </c>
       <c r="I64" t="n">
-        <v>1.818893596775429</v>
+        <v>11.65366083996</v>
       </c>
     </row>
     <row r="65">
@@ -2584,7 +2584,7 @@
         <v>2.121012</v>
       </c>
       <c r="I65" t="n">
-        <v>1.818672046427031</v>
+        <v>11.63772217996</v>
       </c>
     </row>
     <row r="66">
@@ -2617,7 +2617,7 @@
         <v>2.121012</v>
       </c>
       <c r="I66" t="n">
-        <v>1.818226414992708</v>
+        <v>11.60592929996</v>
       </c>
     </row>
     <row r="67">
@@ -2650,7 +2650,7 @@
         <v>2.121009</v>
       </c>
       <c r="I67" t="n">
-        <v>1.817404032428819</v>
+        <v>11.54750929996</v>
       </c>
     </row>
     <row r="68">
@@ -2683,7 +2683,7 @@
         <v>1.939559</v>
       </c>
       <c r="I68" t="n">
-        <v>1.788163666731069</v>
+        <v>9.76632795996</v>
       </c>
     </row>
     <row r="69">
@@ -2716,7 +2716,7 @@
         <v>2.78396</v>
       </c>
       <c r="I69" t="n">
-        <v>1.956703954345838</v>
+        <v>33.16575241996</v>
       </c>
     </row>
     <row r="70">
@@ -2749,7 +2749,7 @@
         <v>2.485646</v>
       </c>
       <c r="I70" t="n">
-        <v>1.953237169491113</v>
+        <v>41.16394051996</v>
       </c>
     </row>
     <row r="71">
@@ -2782,7 +2782,7 @@
         <v>2.242712</v>
       </c>
       <c r="I71" t="n">
-        <v>1.902151521661942</v>
+        <v>21.53758099996</v>
       </c>
     </row>
     <row r="72">
@@ -2815,7 +2815,7 @@
         <v>2.121013</v>
       </c>
       <c r="I72" t="n">
-        <v>1.818893596775429</v>
+        <v>11.65366083996</v>
       </c>
     </row>
     <row r="73">
@@ -2848,7 +2848,7 @@
         <v>2.059153</v>
       </c>
       <c r="I73" t="n">
-        <v>1.713588805558187</v>
+        <v>7.030991089960001</v>
       </c>
     </row>
     <row r="74">
@@ -2881,7 +2881,7 @@
         <v>2.023028</v>
       </c>
       <c r="I74" t="n">
-        <v>1.619220111036396</v>
+        <v>4.98849250996</v>
       </c>
     </row>
     <row r="75">
@@ -2914,7 +2914,7 @@
         <v>1.934502</v>
       </c>
       <c r="I75" t="n">
-        <v>1.48165700843835</v>
+        <v>3.29345817996</v>
       </c>
     </row>
     <row r="76">
@@ -2947,7 +2947,7 @@
         <v>2.120884</v>
       </c>
       <c r="I76" t="n">
-        <v>1.818813880125368</v>
+        <v>11.64876733996</v>
       </c>
     </row>
     <row r="77">
@@ -2980,7 +2980,7 @@
         <v>2.121013</v>
       </c>
       <c r="I77" t="n">
-        <v>1.818893596775429</v>
+        <v>11.65366083996</v>
       </c>
     </row>
     <row r="78">
@@ -3013,7 +3013,7 @@
         <v>2.121122</v>
       </c>
       <c r="I78" t="n">
-        <v>1.818978096568205</v>
+        <v>11.65889467996</v>
       </c>
     </row>
     <row r="79">
@@ -3046,7 +3046,7 @@
         <v>2.121241</v>
       </c>
       <c r="I79" t="n">
-        <v>1.818998541685307</v>
+        <v>11.65931334996</v>
       </c>
     </row>
     <row r="80">
@@ -3079,7 +3079,7 @@
         <v>2.118625</v>
       </c>
       <c r="I80" t="n">
-        <v>1.819064990520892</v>
+        <v>11.66430012996</v>
       </c>
     </row>
     <row r="81">
@@ -3112,7 +3112,7 @@
         <v>2.121013</v>
       </c>
       <c r="I81" t="n">
-        <v>1.818893596775429</v>
+        <v>11.65366083996</v>
       </c>
     </row>
     <row r="82">
@@ -3145,7 +3145,7 @@
         <v>2.121156</v>
       </c>
       <c r="I82" t="n">
-        <v>1.818869442566909</v>
+        <v>11.65199244996</v>
       </c>
     </row>
     <row r="83">
@@ -3178,7 +3178,7 @@
         <v>2.121157</v>
       </c>
       <c r="I83" t="n">
-        <v>1.818869755447212</v>
+        <v>11.65199651996</v>
       </c>
     </row>
     <row r="84">
@@ -3211,7 +3211,7 @@
         <v>2.121013</v>
       </c>
       <c r="I84" t="n">
-        <v>1.818722761707717</v>
+        <v>11.64132725996</v>
       </c>
     </row>
     <row r="85">
@@ -3244,7 +3244,7 @@
         <v>2.121013</v>
       </c>
       <c r="I85" t="n">
-        <v>1.818893596775429</v>
+        <v>11.65366083996</v>
       </c>
     </row>
     <row r="86">
@@ -3277,7 +3277,7 @@
         <v>2.121013</v>
       </c>
       <c r="I86" t="n">
-        <v>1.819168757390788</v>
+        <v>11.67336391996</v>
       </c>
     </row>
     <row r="87">
@@ -3310,7 +3310,7 @@
         <v>2.121013</v>
       </c>
       <c r="I87" t="n">
-        <v>1.818951804196615</v>
+        <v>11.65775287996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>